<commit_message>
Updates and new coupling file
</commit_message>
<xml_diff>
--- a/src/coupling.xlsx
+++ b/src/coupling.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Semester_project_git\2022-msc-sem-proj-nseemann\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEC9420D-6A5A-4655-BDC9-BCED1CD7E026}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBE83E1D-60CF-4D2E-8E93-14D18EC37BA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20640" yWindow="-3960" windowWidth="17250" windowHeight="8865" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="waste_skips_gis" sheetId="1" r:id="rId1"/>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="51">
-  <si>
-    <t>Name</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="69">
   <si>
     <t>long</t>
   </si>
@@ -162,22 +159,79 @@
     <t>Corresponding dump arrivals</t>
   </si>
   <si>
-    <t>Direct skip data</t>
-  </si>
-  <si>
     <t>#</t>
   </si>
   <si>
     <t>none</t>
   </si>
   <si>
-    <t>Bangwe</t>
-  </si>
-  <si>
-    <t>BCA</t>
-  </si>
-  <si>
-    <t>Naizi</t>
+    <t>avg_ramp</t>
+  </si>
+  <si>
+    <t>number_ramps</t>
+  </si>
+  <si>
+    <t>days_overfull_prop</t>
+  </si>
+  <si>
+    <t>Bangwe_Organic_1</t>
+  </si>
+  <si>
+    <t>Bangwe_Organic_2</t>
+  </si>
+  <si>
+    <t>Bangwe_inorganic_1</t>
+  </si>
+  <si>
+    <t>Bangwe_inorganic_2</t>
+  </si>
+  <si>
+    <t>BCA_Organic_1</t>
+  </si>
+  <si>
+    <t>BCA_Organic_2</t>
+  </si>
+  <si>
+    <t>BCA_inorganic_1</t>
+  </si>
+  <si>
+    <t>BCA_inorganic_2</t>
+  </si>
+  <si>
+    <t>Naizi_Organic_1</t>
+  </si>
+  <si>
+    <t>Naizi_inorganic_1</t>
+  </si>
+  <si>
+    <t>Chigumula_Organic_1</t>
+  </si>
+  <si>
+    <t>Chigumula_Organic_2</t>
+  </si>
+  <si>
+    <t>Chigumula_inorganic_1</t>
+  </si>
+  <si>
+    <t>Chigumula_inorganic_2</t>
+  </si>
+  <si>
+    <t>Name (from GPS data)</t>
+  </si>
+  <si>
+    <t>Direct skip data (ramp rates)</t>
+  </si>
+  <si>
+    <t>Naizi_Organic_1, Naizi_Inorganic_1</t>
+  </si>
+  <si>
+    <t>BCA_Organic_1,BCA_Organic_2,BCA_inorganic_1,BCA_inorganic_2</t>
+  </si>
+  <si>
+    <t>Bangwe_Organic_1,Bangwe_inorganic_1,Bangwe_inorganic_2</t>
+  </si>
+  <si>
+    <t>Chigumula_Organic_1,Chigumula_Organic_2,Chigumula_inorganic_1,Chigumula_inorganic_2</t>
   </si>
 </sst>
 </file>
@@ -201,7 +255,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -209,12 +263,101 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -495,46 +638,57 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G54"/>
+  <dimension ref="A1:N54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="22.5546875" customWidth="1"/>
-    <col min="4" max="4" width="26" customWidth="1"/>
+    <col min="4" max="4" width="82.21875" customWidth="1"/>
     <col min="5" max="5" width="10.109375" customWidth="1"/>
     <col min="6" max="6" width="28" customWidth="1"/>
+    <col min="7" max="7" width="12.88671875" customWidth="1"/>
+    <col min="11" max="11" width="23.88671875" customWidth="1"/>
+    <col min="12" max="12" width="12.33203125" customWidth="1"/>
+    <col min="13" max="13" width="14.44140625" customWidth="1"/>
+    <col min="14" max="14" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" t="s">
+        <v>43</v>
+      </c>
+      <c r="L1" t="s">
+        <v>46</v>
+      </c>
+      <c r="M1" t="s">
+        <v>47</v>
+      </c>
+      <c r="N1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E1" t="s">
-        <v>46</v>
-      </c>
-      <c r="F1" t="s">
-        <v>44</v>
-      </c>
-      <c r="G1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>3</v>
       </c>
       <c r="B2">
         <v>35.050629288236699</v>
@@ -543,15 +697,24 @@
         <v>-15.775147819237599</v>
       </c>
       <c r="F2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="L2" s="2">
+        <v>0.21505999787249699</v>
+      </c>
+      <c r="M2" s="2">
+        <v>24</v>
+      </c>
+      <c r="N2" s="3">
+        <v>0.25816023738872401</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>3</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>4</v>
       </c>
       <c r="B3">
         <v>35.014843300000003</v>
@@ -560,15 +723,22 @@
         <v>-15.8270523</v>
       </c>
       <c r="F3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5">
+        <v>1</v>
+      </c>
+      <c r="N3" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>4</v>
-      </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>5</v>
       </c>
       <c r="B4">
         <v>35.088191600000002</v>
@@ -577,18 +747,27 @@
         <v>-15.8496159</v>
       </c>
       <c r="D4" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="F4" t="s">
+        <v>4</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="L4" s="5">
+        <v>0.48964803312629401</v>
+      </c>
+      <c r="M4" s="5">
+        <v>23</v>
+      </c>
+      <c r="N4" s="6">
+        <v>0.72477064220183396</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>5</v>
-      </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>6</v>
       </c>
       <c r="B5">
         <v>35.081051900669301</v>
@@ -597,15 +776,24 @@
         <v>-15.744664723304901</v>
       </c>
       <c r="F5" t="s">
-        <v>47</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="L5" s="8">
+        <v>0.39956597222222201</v>
+      </c>
+      <c r="M5" s="8">
+        <v>16</v>
+      </c>
+      <c r="N5" s="9">
+        <v>0.73725490196078403</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6">
         <v>35.056110506117001</v>
@@ -614,15 +802,24 @@
         <v>-15.7308852158985</v>
       </c>
       <c r="F6" t="s">
+        <v>6</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="L6" s="2">
+        <v>9.1082621525205201E-2</v>
+      </c>
+      <c r="M6" s="2">
+        <v>11</v>
+      </c>
+      <c r="N6" s="3">
+        <v>0.386292834890965</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>7</v>
-      </c>
-      <c r="G6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>8</v>
       </c>
       <c r="B7">
         <v>35.0745535217875</v>
@@ -631,15 +828,24 @@
         <v>-15.7677063561359</v>
       </c>
       <c r="F7" t="s">
+        <v>7</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="L7" s="5">
+        <v>7.67045454545454E-2</v>
+      </c>
+      <c r="M7" s="5">
+        <v>2</v>
+      </c>
+      <c r="N7" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>8</v>
-      </c>
-      <c r="G7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>9</v>
       </c>
       <c r="B8">
         <v>35.076323799999997</v>
@@ -648,15 +854,24 @@
         <v>-15.7904719</v>
       </c>
       <c r="F8" t="s">
+        <v>8</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="L8" s="5">
+        <v>6.3114808212847401E-2</v>
+      </c>
+      <c r="M8" s="5">
+        <v>6</v>
+      </c>
+      <c r="N8" s="6">
+        <v>0.53592814371257402</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>9</v>
-      </c>
-      <c r="G8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>10</v>
       </c>
       <c r="B9">
         <v>35.084111499999999</v>
@@ -665,15 +880,24 @@
         <v>-15.8079213</v>
       </c>
       <c r="F9" t="s">
-        <v>10</v>
-      </c>
-      <c r="G9">
+        <v>9</v>
+      </c>
+      <c r="K9" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="L9" s="8">
+        <v>3.8461538461538401E-2</v>
+      </c>
+      <c r="M9" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="N9" s="9">
+        <v>0.62711864406779605</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10">
         <v>35.105332599999997</v>
@@ -682,15 +906,24 @@
         <v>-15.793434299999999</v>
       </c>
       <c r="F10" t="s">
-        <v>10</v>
-      </c>
-      <c r="G10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="L10" s="2">
+        <v>4.5997124677223299E-2</v>
+      </c>
+      <c r="M10" s="2">
+        <v>8</v>
+      </c>
+      <c r="N10" s="3">
+        <v>0.209876543209876</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B11">
         <v>35.082307399999998</v>
@@ -699,18 +932,27 @@
         <v>-15.849474900000001</v>
       </c>
       <c r="D11" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="F11" t="s">
-        <v>5</v>
-      </c>
-      <c r="G11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+      <c r="K11" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="L11" s="8">
+        <v>0.14449489691594899</v>
+      </c>
+      <c r="M11" s="8">
+        <v>15</v>
+      </c>
+      <c r="N11" s="9">
+        <v>0.292899408284023</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
         <v>35.084882999999998</v>
@@ -719,18 +961,27 @@
         <v>-15.8282683</v>
       </c>
       <c r="D12" t="s">
-        <v>48</v>
+        <v>67</v>
       </c>
       <c r="F12" t="s">
-        <v>11</v>
-      </c>
-      <c r="G12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="L12" s="2">
+        <v>0.15767444506940301</v>
+      </c>
+      <c r="M12" s="2">
+        <v>21</v>
+      </c>
+      <c r="N12" s="3">
+        <v>0.18322981366459601</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B13">
         <v>35.088650999999999</v>
@@ -739,18 +990,27 @@
         <v>-15.8322942</v>
       </c>
       <c r="D13" t="s">
-        <v>48</v>
+        <v>67</v>
       </c>
       <c r="F13" t="s">
-        <v>11</v>
-      </c>
-      <c r="G13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+      <c r="K13" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="L13" s="5">
+        <v>0.12701289095519799</v>
+      </c>
+      <c r="M13" s="5">
+        <v>13</v>
+      </c>
+      <c r="N13" s="6">
+        <v>0.106481481481481</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B14">
         <v>35.092860600000002</v>
@@ -759,18 +1019,27 @@
         <v>-15.8318935</v>
       </c>
       <c r="D14" t="s">
-        <v>48</v>
+        <v>67</v>
       </c>
       <c r="F14" t="s">
+        <v>10</v>
+      </c>
+      <c r="K14" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="L14" s="5">
+        <v>5.5501414876414801E-2</v>
+      </c>
+      <c r="M14" s="5">
+        <v>4</v>
+      </c>
+      <c r="N14" s="6">
+        <v>0.25617283950617198</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>11</v>
-      </c>
-      <c r="G14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>12</v>
       </c>
       <c r="B15">
         <v>35.090235499999999</v>
@@ -779,18 +1048,27 @@
         <v>-15.8162941</v>
       </c>
       <c r="D15" t="s">
-        <v>48</v>
+        <v>67</v>
       </c>
       <c r="F15" t="s">
-        <v>12</v>
-      </c>
-      <c r="G15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+      <c r="K15" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="L15" s="8">
+        <v>0.12833333333333299</v>
+      </c>
+      <c r="M15" s="8">
+        <v>2</v>
+      </c>
+      <c r="N15" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B16">
         <v>35.097234299999997</v>
@@ -799,18 +1077,15 @@
         <v>-15.809099700000001</v>
       </c>
       <c r="D16" t="s">
-        <v>48</v>
+        <v>67</v>
       </c>
       <c r="F16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>12</v>
-      </c>
-      <c r="G16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>13</v>
       </c>
       <c r="B17">
         <v>35.064146399999998</v>
@@ -819,15 +1094,12 @@
         <v>-15.8129183</v>
       </c>
       <c r="F17" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>13</v>
-      </c>
-      <c r="G17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>14</v>
       </c>
       <c r="B18">
         <v>35.054739699999999</v>
@@ -836,15 +1108,12 @@
         <v>-15.820991100000001</v>
       </c>
       <c r="F18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>14</v>
-      </c>
-      <c r="G18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>15</v>
       </c>
       <c r="B19">
         <v>35.04983</v>
@@ -853,15 +1122,12 @@
         <v>-15.8140027</v>
       </c>
       <c r="F19" t="s">
-        <v>15</v>
-      </c>
-      <c r="G19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B20">
         <v>35.058945899999998</v>
@@ -870,15 +1136,12 @@
         <v>-15.812279500000001</v>
       </c>
       <c r="F20" t="s">
-        <v>14</v>
-      </c>
-      <c r="G20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B21">
         <v>35.056525399999998</v>
@@ -887,15 +1150,12 @@
         <v>-15.829165700000001</v>
       </c>
       <c r="F21" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>16</v>
-      </c>
-      <c r="G21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>17</v>
       </c>
       <c r="B22">
         <v>35.056732895464201</v>
@@ -904,15 +1164,12 @@
         <v>-15.853939420484799</v>
       </c>
       <c r="F22" t="s">
-        <v>47</v>
-      </c>
-      <c r="G22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B23">
         <v>35.060600899999997</v>
@@ -921,15 +1178,12 @@
         <v>-15.8204747</v>
       </c>
       <c r="F23" t="s">
-        <v>47</v>
-      </c>
-      <c r="G23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B24">
         <v>35.051785700000003</v>
@@ -938,18 +1192,15 @@
         <v>-15.886139699999999</v>
       </c>
       <c r="D24" t="s">
-        <v>19</v>
+        <v>68</v>
       </c>
       <c r="F24" t="s">
-        <v>47</v>
-      </c>
-      <c r="G24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B25">
         <v>35.044387499999999</v>
@@ -958,18 +1209,15 @@
         <v>-15.8874332</v>
       </c>
       <c r="D25" t="s">
+        <v>68</v>
+      </c>
+      <c r="F25" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
         <v>19</v>
-      </c>
-      <c r="F25" t="s">
-        <v>47</v>
-      </c>
-      <c r="G25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>20</v>
       </c>
       <c r="B26">
         <v>35.0630205</v>
@@ -978,18 +1226,15 @@
         <v>-15.8441823</v>
       </c>
       <c r="D26" t="s">
-        <v>49</v>
+        <v>66</v>
       </c>
       <c r="F26" t="s">
-        <v>20</v>
-      </c>
-      <c r="G26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B27">
         <v>35.069350100000001</v>
@@ -998,18 +1243,15 @@
         <v>-15.8444313</v>
       </c>
       <c r="D27" t="s">
-        <v>49</v>
+        <v>66</v>
       </c>
       <c r="F27" t="s">
-        <v>20</v>
-      </c>
-      <c r="G27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B28">
         <v>35.064882500000003</v>
@@ -1018,18 +1260,15 @@
         <v>-15.8486964</v>
       </c>
       <c r="D28" t="s">
-        <v>49</v>
+        <v>66</v>
       </c>
       <c r="F28" t="s">
-        <v>20</v>
-      </c>
-      <c r="G28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B29">
         <v>35.050655900000002</v>
@@ -1038,18 +1277,15 @@
         <v>-15.8929361</v>
       </c>
       <c r="D29" t="s">
-        <v>19</v>
+        <v>68</v>
       </c>
       <c r="F29" t="s">
-        <v>47</v>
-      </c>
-      <c r="G29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B30">
         <v>35.047725715194602</v>
@@ -1058,15 +1294,12 @@
         <v>-15.776765800689899</v>
       </c>
       <c r="F30" t="s">
-        <v>3</v>
-      </c>
-      <c r="G30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B31">
         <v>35.036799031737402</v>
@@ -1075,15 +1308,12 @@
         <v>-15.7768339217149</v>
       </c>
       <c r="F31" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
         <v>21</v>
-      </c>
-      <c r="G31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>22</v>
       </c>
       <c r="B32">
         <v>35.017316800000003</v>
@@ -1092,15 +1322,12 @@
         <v>-15.730363000000001</v>
       </c>
       <c r="F32" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
         <v>22</v>
-      </c>
-      <c r="G32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>23</v>
       </c>
       <c r="B33">
         <v>35.019198287737503</v>
@@ -1109,15 +1336,12 @@
         <v>-15.744681227153199</v>
       </c>
       <c r="F33" t="s">
-        <v>23</v>
-      </c>
-      <c r="G33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B34">
         <v>35.0220263</v>
@@ -1126,15 +1350,12 @@
         <v>-15.744324199999999</v>
       </c>
       <c r="F34" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
         <v>23</v>
-      </c>
-      <c r="G34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>24</v>
       </c>
       <c r="B35">
         <v>35.010177017063398</v>
@@ -1143,15 +1364,12 @@
         <v>-15.746731102769299</v>
       </c>
       <c r="F35" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
         <v>24</v>
-      </c>
-      <c r="G35">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>25</v>
       </c>
       <c r="B36">
         <v>34.999359508364698</v>
@@ -1160,15 +1378,12 @@
         <v>-15.7660058949426</v>
       </c>
       <c r="F36" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
         <v>25</v>
-      </c>
-      <c r="G36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>26</v>
       </c>
       <c r="B37">
         <v>35.002675640453198</v>
@@ -1177,15 +1392,12 @@
         <v>-15.775749523888701</v>
       </c>
       <c r="F37" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
         <v>26</v>
-      </c>
-      <c r="G37">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>27</v>
       </c>
       <c r="B38">
         <v>35.008046518043699</v>
@@ -1194,15 +1406,12 @@
         <v>-15.775960258767499</v>
       </c>
       <c r="F38" t="s">
-        <v>47</v>
-      </c>
-      <c r="G38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B39">
         <v>34.994528122911497</v>
@@ -1211,15 +1420,12 @@
         <v>-15.770725548667</v>
       </c>
       <c r="F39" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
         <v>28</v>
-      </c>
-      <c r="G39">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>29</v>
       </c>
       <c r="B40">
         <v>34.981716010950599</v>
@@ -1228,15 +1434,12 @@
         <v>-15.773443927770501</v>
       </c>
       <c r="F40" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
         <v>29</v>
-      </c>
-      <c r="G40">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>30</v>
       </c>
       <c r="B41">
         <v>34.983139199999997</v>
@@ -1245,15 +1448,12 @@
         <v>-15.7759035</v>
       </c>
       <c r="F41" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
         <v>30</v>
-      </c>
-      <c r="G41">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>31</v>
       </c>
       <c r="B42">
         <v>34.9799853598876</v>
@@ -1262,15 +1462,12 @@
         <v>-15.7638099660559</v>
       </c>
       <c r="F42" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
         <v>31</v>
-      </c>
-      <c r="G42">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>32</v>
       </c>
       <c r="B43">
         <v>35.006406154460898</v>
@@ -1279,15 +1476,12 @@
         <v>-15.7886359879959</v>
       </c>
       <c r="F43" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
         <v>32</v>
-      </c>
-      <c r="G43">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>33</v>
       </c>
       <c r="B44">
         <v>35.0089775</v>
@@ -1296,15 +1490,12 @@
         <v>-15.7885589</v>
       </c>
       <c r="F44" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
         <v>33</v>
-      </c>
-      <c r="G44">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>34</v>
       </c>
       <c r="B45">
         <v>35.008792700000001</v>
@@ -1313,15 +1504,12 @@
         <v>-15.7944906</v>
       </c>
       <c r="F45" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
         <v>34</v>
-      </c>
-      <c r="G45">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>35</v>
       </c>
       <c r="B46">
         <v>34.991879048965501</v>
@@ -1330,15 +1518,12 @@
         <v>-15.8102664651841</v>
       </c>
       <c r="F46" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
         <v>35</v>
-      </c>
-      <c r="G46">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>36</v>
       </c>
       <c r="B47">
         <v>34.993304526006803</v>
@@ -1347,15 +1532,12 @@
         <v>-15.8120182606814</v>
       </c>
       <c r="F47" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
         <v>36</v>
-      </c>
-      <c r="G47">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
-        <v>37</v>
       </c>
       <c r="B48">
         <v>35.005719672087899</v>
@@ -1364,15 +1546,12 @@
         <v>-15.8324505806528</v>
       </c>
       <c r="F48" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
         <v>37</v>
-      </c>
-      <c r="G48">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
-        <v>38</v>
       </c>
       <c r="B49">
         <v>35.011705800000001</v>
@@ -1381,15 +1560,12 @@
         <v>-15.8196523</v>
       </c>
       <c r="F49" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
         <v>38</v>
-      </c>
-      <c r="G49">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
-        <v>39</v>
       </c>
       <c r="B50">
         <v>35.017745599999998</v>
@@ -1398,15 +1574,12 @@
         <v>-15.8164725</v>
       </c>
       <c r="F50" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
         <v>39</v>
-      </c>
-      <c r="G50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
-        <v>40</v>
       </c>
       <c r="B51">
         <v>35.008294999999997</v>
@@ -1415,15 +1588,12 @@
         <v>-15.8154094</v>
       </c>
       <c r="F51" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
         <v>40</v>
-      </c>
-      <c r="G51">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
-        <v>41</v>
       </c>
       <c r="B52">
         <v>35.015308328047801</v>
@@ -1432,15 +1602,12 @@
         <v>-15.8093981762749</v>
       </c>
       <c r="F52" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
         <v>41</v>
-      </c>
-      <c r="G52">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
-        <v>42</v>
       </c>
       <c r="B53">
         <v>35.015760197301198</v>
@@ -1449,15 +1616,12 @@
         <v>-15.7856834240139</v>
       </c>
       <c r="F53" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
         <v>42</v>
-      </c>
-      <c r="G53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
-        <v>43</v>
       </c>
       <c r="B54">
         <v>35.019052113496599</v>
@@ -1466,10 +1630,7 @@
         <v>-15.802852583209001</v>
       </c>
       <c r="F54" t="s">
-        <v>43</v>
-      </c>
-      <c r="G54">
-        <v>1</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding Gantt, update GIS, update Scripts
</commit_message>
<xml_diff>
--- a/src/coupling.xlsx
+++ b/src/coupling.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Semester_project_git\2022-msc-sem-proj-nseemann\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBE83E1D-60CF-4D2E-8E93-14D18EC37BA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FAC403D-789C-458F-BEDA-1D5A0E516523}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -641,7 +641,7 @@
   <dimension ref="A1:N54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>